<commit_message>
MC1.1 & TGM tweaks
Tweaked MC1.1 to improve prints
TGM PBS updated,
</commit_message>
<xml_diff>
--- a/LoRa Base Station/LBS Mk1 PBS.xlsx
+++ b/LoRa Base Station/LBS Mk1 PBS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Storage\Documents\GitHub\Trak-TFRC-System\LoRa Base Station\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A79A401-3EB3-44C1-9CCB-1ECABDE7A2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130AE8EA-7F46-4D8F-A4C5-F90F54BB1085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="162">
   <si>
     <t>Pricing</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Order Qty.</t>
-  </si>
-  <si>
-    <t>Stage</t>
   </si>
   <si>
     <t>Remarks</t>
@@ -581,6 +578,21 @@
   </si>
   <si>
     <t>LoRa Base Station 1.2 - Product Breakdown Sheet</t>
+  </si>
+  <si>
+    <t>LT1A01-024</t>
+  </si>
+  <si>
+    <t>M4 Wingnut</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>Guptas</t>
+  </si>
+  <si>
+    <t>Wingbolts can be used too to replace three M4x14 bolts used for the covers.</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,18 +1111,17 @@
     <col min="6" max="6" width="23.140625" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="49.42578125" customWidth="1"/>
+    <col min="9" max="9" width="42.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1120,18 +1131,17 @@
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
       <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28" t="s">
+      <c r="J1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="1"/>
-      <c r="O1" s="29" t="s">
+      <c r="K1" s="28"/>
+      <c r="L1" s="1"/>
+      <c r="N1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="30"/>
-    </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1161,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>8</v>
@@ -1159,7 +1169,7 @@
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="5" t="s">
@@ -1168,22 +1178,19 @@
       <c r="L2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -1195,30 +1202,27 @@
       <c r="H3" s="15">
         <v>40</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16">
+        <f>SUM(K4:K30)</f>
+        <v>8132.3877276867042</v>
+      </c>
+      <c r="L3" s="16">
+        <f>SUM(L4:L43)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="17"/>
+      <c r="O3" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>15</v>
-      </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16">
-        <f>SUM(L4:L29)</f>
-        <v>8126.3877276867042</v>
-      </c>
-      <c r="M3" s="16">
-        <f>SUM(M4:M43)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -1226,1200 +1230,1122 @@
       <c r="F4" s="12"/>
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="17"/>
+      <c r="O4" s="17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="9">
         <v>1</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>17</v>
+      <c r="J5" s="16">
+        <v>1600</v>
       </c>
       <c r="K5" s="16">
+        <f>G5*J5</f>
         <v>1600</v>
       </c>
-      <c r="L5" s="16">
-        <f>G5*K5</f>
-        <v>1600</v>
-      </c>
-      <c r="M5" s="16"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="16"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="9">
         <v>1</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="K6" s="16">
+      <c r="I6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="16">
         <f>100/122+15</f>
         <v>15.819672131147541</v>
       </c>
-      <c r="L6" s="16">
-        <f t="shared" ref="L6:L27" si="0">G6*K6</f>
+      <c r="K6" s="16">
+        <f>G6*J6</f>
         <v>15.819672131147541</v>
       </c>
-      <c r="M6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="N6" s="17" t="s">
+        <v>3</v>
+      </c>
       <c r="O6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7" s="9">
         <v>1</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>120</v>
+      <c r="I7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="J7" s="16">
+        <v>50</v>
       </c>
       <c r="K7" s="16">
+        <f>G7*J7</f>
         <v>50</v>
       </c>
-      <c r="L7" s="16">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="M7" s="16"/>
-      <c r="O7" s="17" t="s">
+      <c r="L7" s="16"/>
+      <c r="N7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="P7" s="17"/>
-    </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G8" s="9">
         <v>2</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>120</v>
+      <c r="I8" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="J8" s="16">
+        <v>300</v>
       </c>
       <c r="K8" s="16">
-        <v>300</v>
-      </c>
-      <c r="L8" s="16">
-        <f t="shared" si="0"/>
+        <f>G8*J8</f>
         <v>600</v>
       </c>
-      <c r="M8" s="16"/>
-      <c r="O8" s="17" t="s">
+      <c r="L8" s="16"/>
+      <c r="N8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O8" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G9" s="9">
         <v>1</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>17</v>
+      <c r="J9" s="16">
+        <v>800</v>
       </c>
       <c r="K9" s="16">
+        <f>G9*J9</f>
         <v>800</v>
       </c>
-      <c r="L9" s="16">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="M9" s="16"/>
-      <c r="O9" s="17" t="s">
+      <c r="L9" s="16"/>
+      <c r="N9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>106</v>
       </c>
       <c r="G10" s="9">
         <v>1</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="16">
+      <c r="J10" s="16">
         <f>700/63</f>
         <v>11.111111111111111</v>
       </c>
-      <c r="L10" s="16">
-        <f t="shared" si="0"/>
+      <c r="K10" s="16">
+        <f>G10*J10</f>
         <v>11.111111111111111</v>
       </c>
-      <c r="M10" s="16"/>
-      <c r="O10" s="17" t="s">
+      <c r="L10" s="16"/>
+      <c r="N10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="P10" s="20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O10" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>45</v>
-      </c>
       <c r="F11" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" s="9">
         <v>1</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="K11" s="16">
+      <c r="I11" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" s="16">
         <f>2500/10+4338</f>
         <v>4588</v>
       </c>
-      <c r="L11" s="16">
-        <f t="shared" si="0"/>
+      <c r="K11" s="16">
+        <f>G11*J11</f>
         <v>4588</v>
       </c>
-      <c r="M11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="N11" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="O11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="P11" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G12" s="9">
         <v>1</v>
       </c>
-      <c r="I12" s="12" t="s">
-        <v>34</v>
+      <c r="J12" s="16">
+        <v>17</v>
       </c>
       <c r="K12" s="16">
+        <f>G12*J12</f>
         <v>17</v>
       </c>
-      <c r="L12" s="16">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="M12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="N12" s="17" t="s">
+        <v>24</v>
+      </c>
       <c r="O12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="P12" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G13" s="9">
         <v>2</v>
       </c>
-      <c r="I13" s="12" t="s">
-        <v>17</v>
+      <c r="J13" s="16">
+        <v>3.3</v>
       </c>
       <c r="K13" s="16">
-        <v>3.3</v>
-      </c>
-      <c r="L13" s="16">
-        <f t="shared" si="0"/>
+        <f>G13*J13</f>
         <v>6.6</v>
       </c>
-      <c r="M13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="N13" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="O13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="P13" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G14" s="9">
         <v>1</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="16">
+      <c r="J14" s="16">
         <f>211/36+30</f>
         <v>35.861111111111114</v>
       </c>
-      <c r="L14" s="16">
-        <f t="shared" si="0"/>
+      <c r="K14" s="16">
+        <f>G14*J14</f>
         <v>35.861111111111114</v>
       </c>
-      <c r="M14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="N14" s="17" t="s">
+        <v>9</v>
+      </c>
       <c r="O14" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="P14" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>106</v>
       </c>
       <c r="G15" s="9">
         <v>1</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>17</v>
+      <c r="J15" s="16">
+        <v>5</v>
       </c>
       <c r="K15" s="16">
+        <f>G15*J15</f>
         <v>5</v>
       </c>
-      <c r="L15" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="M15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="N15" s="17"/>
       <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-    </row>
-    <row r="16" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="9">
         <v>1</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="16">
+      <c r="J16" s="16">
         <f>211/48+30</f>
         <v>34.395833333333336</v>
       </c>
-      <c r="L16" s="16">
-        <f t="shared" si="0"/>
+      <c r="K16" s="16">
+        <f>G16*J16</f>
         <v>34.395833333333336</v>
       </c>
-      <c r="M16" s="16"/>
-      <c r="O16" s="10" t="s">
+      <c r="L16" s="16"/>
+      <c r="N16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="P16" s="17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>106</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>17</v>
+      <c r="J17" s="16">
+        <v>4</v>
       </c>
       <c r="K17" s="16">
+        <f>G17*J17</f>
         <v>4</v>
       </c>
-      <c r="L17" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="M17" s="16"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="16"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="J18" s="16">
+        <v>79</v>
+      </c>
+      <c r="K18" s="16">
+        <f>G18*J18</f>
+        <v>79</v>
+      </c>
+      <c r="L18" s="16"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="16">
-        <v>79</v>
-      </c>
-      <c r="L18" s="16">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="M18" s="16"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="E19" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="J19" s="16">
+        <v>16</v>
+      </c>
+      <c r="K19" s="16">
+        <f>G19*J19</f>
+        <v>16</v>
+      </c>
+      <c r="L19" s="16"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="16">
-        <v>16</v>
-      </c>
-      <c r="L19" s="16">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="M19" s="16"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20" s="9">
         <v>5</v>
       </c>
-      <c r="I20" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="21">
+      <c r="J20" s="21">
         <v>1</v>
       </c>
-      <c r="L20" s="16">
-        <f t="shared" si="0"/>
+      <c r="K20" s="16">
+        <f>G20*J20</f>
         <v>5</v>
       </c>
-      <c r="M20" s="16"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="16"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="9">
         <v>10</v>
       </c>
-      <c r="I21" s="12" t="s">
-        <v>35</v>
+      <c r="J21" s="16">
+        <v>6.6</v>
       </c>
       <c r="K21" s="16">
-        <v>6.6</v>
-      </c>
-      <c r="L21" s="16">
-        <f t="shared" si="0"/>
+        <f>G21*J21</f>
         <v>66</v>
       </c>
-      <c r="M21" s="16"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="17" t="s">
+      <c r="L21" s="16"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="D22" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22" s="9">
         <v>10</v>
       </c>
-      <c r="I22" s="12" t="s">
-        <v>35</v>
+      <c r="J22" s="16">
+        <v>1.5</v>
       </c>
       <c r="K22" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="L22" s="16">
-        <f t="shared" si="0"/>
+        <f>G22*J22</f>
         <v>15</v>
       </c>
-      <c r="M22" s="16"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="16"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G23" s="9">
         <v>3</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I23" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" s="16">
+        <v>2</v>
+      </c>
+      <c r="K23" s="16">
+        <f>G23*J23</f>
+        <v>6</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="K23" s="16">
-        <v>2</v>
-      </c>
-      <c r="L23" s="16">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="M23" s="16"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>148</v>
-      </c>
       <c r="E24" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G24" s="9">
         <v>10</v>
       </c>
-      <c r="I24" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>128</v>
+      <c r="I24" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J24" s="16">
+        <v>2</v>
       </c>
       <c r="K24" s="16">
-        <v>2</v>
-      </c>
-      <c r="L24" s="16">
-        <f t="shared" si="0"/>
+        <f>G24*J24</f>
         <v>20</v>
       </c>
-      <c r="M24" s="16"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="16"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G25" s="9">
         <v>4</v>
       </c>
-      <c r="I25" s="12" t="s">
-        <v>35</v>
+      <c r="J25" s="16">
+        <v>0.9</v>
       </c>
       <c r="K25" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="L25" s="16">
-        <f t="shared" si="0"/>
+        <f>G25*J25</f>
         <v>3.6</v>
       </c>
+      <c r="N25" s="17"/>
       <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-    </row>
-    <row r="26" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G26" s="9">
         <v>4</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>142</v>
+      <c r="I26" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="16">
+        <v>3</v>
       </c>
       <c r="K26" s="16">
-        <v>3</v>
-      </c>
-      <c r="L26" s="16">
-        <f t="shared" si="0"/>
+        <f>G26*J26</f>
         <v>12</v>
       </c>
-      <c r="O26" s="10" t="s">
+      <c r="N26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="P26" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>138</v>
-      </c>
       <c r="C27" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G27" s="9">
         <v>4</v>
       </c>
-      <c r="I27" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>142</v>
+      <c r="I27" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="16">
+        <v>2</v>
       </c>
       <c r="K27" s="16">
+        <f>G27*J27</f>
+        <v>8</v>
+      </c>
+      <c r="L27" s="16"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="9">
+        <v>3</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J28" s="16">
         <v>2</v>
       </c>
-      <c r="L27" s="16">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M27" s="16"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17" t="s">
+      <c r="K28" s="16">
+        <f>G28*J28</f>
+        <v>6</v>
+      </c>
+      <c r="L28" s="16"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="22"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E28" s="22"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="9">
+      <c r="D30" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="9">
         <v>1</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K29" s="16">
+      <c r="J30" s="16">
         <f>98+30</f>
         <v>128</v>
       </c>
-      <c r="L29" s="16">
-        <f>G29*K29</f>
+      <c r="K30" s="16">
+        <f>G30*J30</f>
         <v>128</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="G30" s="9">
+      <c r="L30" s="16"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="9">
         <v>1</v>
       </c>
-      <c r="I30" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" s="16">
+      <c r="J31" s="16">
         <f>600/36+25</f>
         <v>41.666666666666671</v>
       </c>
-      <c r="L30" s="16">
-        <f>G30*K30</f>
+      <c r="K31" s="16">
+        <f>G31*J31</f>
         <v>41.666666666666671</v>
       </c>
-      <c r="M30" s="16"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17" t="s">
+      <c r="L31" s="16"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E31" s="22"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17" t="s">
+    <row r="32" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="22"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+    <row r="33" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="9">
+        <v>1</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16">
+        <f>G33*J33</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="16"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="G32" s="9">
-        <v>1</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="J32" s="9" t="s">
+      <c r="B34" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16">
-        <f>G32*K32</f>
-        <v>0</v>
-      </c>
-      <c r="M32" s="16"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G33" s="9">
-        <v>4</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K33" s="16">
-        <v>4.8</v>
-      </c>
-      <c r="L33" s="16">
-        <f>G33*K33</f>
-        <v>19.2</v>
-      </c>
-      <c r="M33" s="16"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17" t="s">
+      <c r="E34" s="19" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="G34" s="9">
         <v>4</v>
       </c>
-      <c r="I34" s="12" t="s">
-        <v>35</v>
+      <c r="J34" s="16">
+        <v>4.8</v>
       </c>
       <c r="K34" s="16">
-        <v>1.6</v>
-      </c>
-      <c r="L34" s="16">
-        <f>G34*K34</f>
-        <v>6.4</v>
-      </c>
-      <c r="M34" s="16"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>G34*J34</f>
+        <v>19.2</v>
+      </c>
+      <c r="L34" s="16"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G35" s="9">
         <v>4</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="J35" s="16">
+        <v>1.6</v>
+      </c>
+      <c r="K35" s="16">
+        <f>G35*J35</f>
+        <v>6.4</v>
+      </c>
+      <c r="L35" s="16"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K35" s="16">
+      <c r="D36" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="9">
+        <v>4</v>
+      </c>
+      <c r="J36" s="16">
         <v>3</v>
       </c>
-      <c r="L35" s="16">
-        <f>G35*K35</f>
+      <c r="K36" s="16">
+        <f>G36*J36</f>
         <v>12</v>
       </c>
-      <c r="M35" s="16"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="E36" s="19"/>
-      <c r="I36" s="12"/>
-      <c r="K36" s="16"/>
       <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
+      <c r="N36" s="17"/>
       <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-    </row>
-    <row r="37" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
-      <c r="B37" s="23" t="s">
-        <v>151</v>
-      </c>
       <c r="E37" s="19"/>
-      <c r="I37" s="12"/>
+      <c r="J37" s="16"/>
       <c r="K37" s="16"/>
       <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
+      <c r="N37" s="17"/>
       <c r="O37" s="17"/>
-      <c r="P37" s="17"/>
-    </row>
-    <row r="38" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B38" s="9" t="s">
+    </row>
+    <row r="38" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12"/>
+      <c r="B38" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="G38" s="9">
+      <c r="E39" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" s="9">
         <v>1</v>
       </c>
-      <c r="I38" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K38" s="16">
+      <c r="J39" s="16">
         <f>30</f>
         <v>30</v>
       </c>
-      <c r="L38" s="16">
-        <f>G38*K38</f>
+      <c r="K39" s="16">
+        <f>G39*J39</f>
         <v>30</v>
       </c>
-      <c r="M38" s="16"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="9" t="s">
+      <c r="L39" s="16"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="G39" s="9">
+      <c r="E40" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9">
         <v>1</v>
       </c>
-      <c r="I39" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K39" s="16">
-        <v>25</v>
-      </c>
-      <c r="L39" s="16">
-        <f>G39*K39</f>
-        <v>25</v>
-      </c>
-      <c r="M39" s="16"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="16"/>
+      <c r="J40" s="16">
+        <v>25</v>
+      </c>
+      <c r="K40" s="16">
+        <f>G40*J40</f>
+        <v>25</v>
+      </c>
       <c r="L40" s="16"/>
-      <c r="M40" s="16"/>
+      <c r="N40" s="8"/>
       <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-    </row>
-    <row r="41" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
-      <c r="B41" s="24" t="s">
-        <v>65</v>
-      </c>
+      <c r="B41" s="9"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -2427,154 +2353,162 @@
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
+      <c r="J41" s="16"/>
       <c r="K41" s="16"/>
       <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
-      <c r="O41" s="6" t="s">
+      <c r="N41" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P41" s="8" t="s">
+      <c r="O41" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="7"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9">
+      <c r="C43" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9">
         <v>0.05</v>
       </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J42" s="9"/>
-      <c r="K42" s="16">
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="16">
         <v>320</v>
       </c>
-      <c r="L42" s="16">
-        <f>G42*K42</f>
+      <c r="K43" s="16">
+        <f>G43*J43</f>
         <v>16</v>
       </c>
-      <c r="M42" s="7"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8" t="s">
+      <c r="L43" s="7"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="25" t="s">
-        <v>143</v>
-      </c>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="26" t="s">
-        <v>144</v>
-      </c>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N46" s="8"/>
+      <c r="O46" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="26" t="s">
-        <v>145</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="J47" s="7"/>
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
-      <c r="M47" s="7"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N47" s="8"/>
+      <c r="O47" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="26" t="s">
-        <v>146</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="11:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N48" s="8"/>
+      <c r="O48" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="J49" s="7"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
-      <c r="M49" s="7"/>
+      <c r="N49" s="8"/>
       <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I42 I29:I30 I3:I27 I32:I39" xr:uid="{DEAB30BA-0051-4580-A569-94DA08E24ED1}">
-      <formula1>$P$16:$P$24</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30 C5:C28 C33:C38" xr:uid="{92AF5C1A-EEEA-40CC-898F-63EE0B5887DC}">
+      <formula1>$O$26:$O$33</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C27 C29 C32:C37" xr:uid="{92AF5C1A-EEEA-40CC-898F-63EE0B5887DC}">
-      <formula1>$P$26:$P$33</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E43 E5:E40" xr:uid="{5681D413-582B-4FD5-90BE-0C0E8F568CA9}">
+      <formula1>$O$41:$O$48</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E42 E5:E39" xr:uid="{5681D413-582B-4FD5-90BE-0C0E8F568CA9}">
-      <formula1>$P$41:$P$48</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31" xr:uid="{F3CE9DBF-0220-4C70-AB73-0B881E08D07F}">
+      <formula1>$O$26:$O$34</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30" xr:uid="{F3CE9DBF-0220-4C70-AB73-0B881E08D07F}">
-      <formula1>$P$26:$P$34</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C38:C39" xr:uid="{8B190038-F8EE-45D1-AF16-B64E8BA44894}">
-      <formula1>$P$26:$P$35</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C39:C40" xr:uid="{8B190038-F8EE-45D1-AF16-B64E8BA44894}">
+      <formula1>$O$26:$O$35</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B46" r:id="rId1" xr:uid="{735E7525-90C0-458B-89E1-B4B4F416A965}"/>
-    <hyperlink ref="B47" r:id="rId2" xr:uid="{417DC8E5-C52F-4CD9-A091-A3BF04D1DB99}"/>
-    <hyperlink ref="B48" r:id="rId3" display="https://www.sunrom.com/p/pcb-spacers-6mm-height" xr:uid="{97FD2598-3045-429F-B93F-7546FF742C08}"/>
+    <hyperlink ref="B47" r:id="rId1" xr:uid="{735E7525-90C0-458B-89E1-B4B4F416A965}"/>
+    <hyperlink ref="B48" r:id="rId2" xr:uid="{417DC8E5-C52F-4CD9-A091-A3BF04D1DB99}"/>
+    <hyperlink ref="B49" r:id="rId3" display="https://www.sunrom.com/p/pcb-spacers-6mm-height" xr:uid="{97FD2598-3045-429F-B93F-7546FF742C08}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>

</xml_diff>